<commit_message>
feat: Add Stash plugin integration and comprehensive enhancements
Add complete Stash plugin implementation with batch processing, metadata comparison, and scene transformation capabilities. Enhance parser dictionaries with expanded studio codes, quality markers, and junk token filters. Add configuration system and validation tools. Remove deprecated evaluation metrics and planning documents.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/ref/master.xlsx
+++ b/ref/master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbmiles/Projects/plugin/filename-parser/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B65E8E2-D6CC-7848-B67C-064A54FF0FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52262E9-8594-FA47-BEE1-05E3DF8578EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="137">
   <si>
     <t>input</t>
   </si>
@@ -136,27 +136,6 @@
     <t>{"title": 2}</t>
   </si>
   <si>
-    <t>[3D SBS]SexScenes-Primetime 1080P-Austin, Jack and Alex.mp4</t>
-  </si>
-  <si>
-    <t>.mp4(extension_mp4) | 1080P(resolution_1080P) | 3D SBS(format_3D SBS)</t>
-  </si>
-  <si>
-    <t>SexScenes-Primetime -Austin, Jack and Alex</t>
-  </si>
-  <si>
-    <t>{text}-{text} -{performers}</t>
-  </si>
-  <si>
-    <t>Austin, Jack, Alex</t>
-  </si>
-  <si>
-    <t>{"SexScenes","Primetime"}</t>
-  </si>
-  <si>
-    <t>{"path_tokens": 0, "filename_tokens": 3, "matched_tokens": 1, "match_rate": 0.33}</t>
-  </si>
-  <si>
     <t>[Bare Adventures] Mark Brown &amp; Kevin Ateah.mp4</t>
   </si>
   <si>
@@ -268,9 +247,6 @@
     <t>[Crunchboy] 2 potes d'enfance dans la même bain (movie)</t>
   </si>
   <si>
-    <t>{studio} {text}</t>
-  </si>
-  <si>
     <t>[{studio}] title ({junk})</t>
   </si>
   <si>
@@ -280,12 +256,6 @@
     <t>2 potes d'enfance dans la même bain</t>
   </si>
   <si>
-    <t>{"PART 1"}</t>
-  </si>
-  <si>
-    <t>{"path_tokens": 2, "filename_tokens": 3, "matched_tokens": 4, "match_rate": 0.8}</t>
-  </si>
-  <si>
     <t>Hard Brit Lads 7 of 7/Theo Reid &amp; Scott Hunter.mp4</t>
   </si>
   <si>
@@ -301,12 +271,6 @@
     <t>Theo Reid, Scott Hunter</t>
   </si>
   <si>
-    <t>{"7 of 7"}</t>
-  </si>
-  <si>
-    <t>{"path_tokens": 2, "filename_tokens": 1, "matched_tokens": 2, "match_rate": 0.66}</t>
-  </si>
-  <si>
     <t>Hard Brit Lads 7 of 7/Tom Long, Luke Vogel &amp; AJ Alexander.mp4</t>
   </si>
   <si>
@@ -376,12 +340,6 @@
     <t>{"scene": 2}</t>
   </si>
   <si>
-    <t>{"Collection 1080p"}</t>
-  </si>
-  <si>
-    <t>{"path_tokens": 2, "filename_tokens": 4, "matched_tokens": 5, "match_rate": 0.8}</t>
-  </si>
-  <si>
     <t>TF Part 1 (Individual Scenes)/Julian Ocean &amp; Diego Humbol.mp4</t>
   </si>
   <si>
@@ -391,15 +349,6 @@
     <t>Julian Ocean &amp; Diego Humbol</t>
   </si>
   <si>
-    <t>{text} ({text})</t>
-  </si>
-  <si>
-    <t>{"TF Part 1", "Individual Scenes"}</t>
-  </si>
-  <si>
-    <t>{"path_tokens": 2, "filename_tokens": 1, "matched_tokens": 1, "match_rate": 0.33}</t>
-  </si>
-  <si>
     <t>TIM Classics Collection Part1/Bones For Cumpuppy/Scene 1-Cumpuppy Takes Three Loads.mp4</t>
   </si>
   <si>
@@ -409,9 +358,6 @@
     <t>Scene 1-Cumpuppy Takes Three Loads</t>
   </si>
   <si>
-    <t>{studio} {text}/{group}</t>
-  </si>
-  <si>
     <t>{sequence}-{title}</t>
   </si>
   <si>
@@ -427,12 +373,6 @@
     <t>Bones For Cumpuppy</t>
   </si>
   <si>
-    <t>{"Classics Collection Part1"}</t>
-  </si>
-  <si>
-    <t>{"path_tokens": 3, "filename_tokens": 2, "matched_tokens": 4, "match_rate": 0.8}</t>
-  </si>
-  <si>
     <t>TIM Classics Collection Part1/Cum Whore/Scene 5-Peto Coast, Steven Daigle, And Marcus Isaacs.mp4</t>
   </si>
   <si>
@@ -452,6 +392,45 @@
   </si>
   <si>
     <t>Cum Whore</t>
+  </si>
+  <si>
+    <t>(2005) Eurocreme - RAW Films - Raw Edge (720p)).mp4</t>
+  </si>
+  <si>
+    <t>.mp4(extension_mp4) | 720p(resolution_720p)</t>
+  </si>
+  <si>
+    <t>(2005) Eurocreme - RAW Films - Raw Edge</t>
+  </si>
+  <si>
+    <t>({date}) {studio} - {line} - {title}</t>
+  </si>
+  <si>
+    <t>Raw Edge</t>
+  </si>
+  <si>
+    <t>{"path_tokens": 0, "filename_tokens": 4, "matched_tokens": 4, "match_rate": 1.0}</t>
+  </si>
+  <si>
+    <t>{studio} {junk}</t>
+  </si>
+  <si>
+    <t>{"path_tokens": 2, "filename_tokens": 3, "matched_tokens": 5, "match_rate": 1.0}</t>
+  </si>
+  <si>
+    <t>{"path_tokens": 2, "filename_tokens": 1, "matched_tokens": 3, "match_rate": 1.0}</t>
+  </si>
+  <si>
+    <t>{junk} ({junk})</t>
+  </si>
+  <si>
+    <t>{studio} {junk}/{group}</t>
+  </si>
+  <si>
+    <t>{"path_tokens": 2, "filename_tokens": 4, "matched_tokens": 6, "match_rate": 1.0}</t>
+  </si>
+  <si>
+    <t>{"path_tokens": 3, "filename_tokens": 2, "matched_tokens": 5, "match_rate": 1.0}</t>
   </si>
 </sst>
 </file>
@@ -496,9 +475,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -517,7 +494,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -528,6 +549,31 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BECE464C-B18C-CE41-A884-FBC43B7DCFE5}" name="Table1" displayName="Table1" ref="A1:P21" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:P21" xr:uid="{BECE464C-B18C-CE41-A884-FBC43B7DCFE5}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{C0052427-1D71-6E48-9FBE-442E514BB5B8}" name="input"/>
+    <tableColumn id="2" xr3:uid="{FDD54577-F53D-354F-9AC9-D55286E37EED}" name="removed"/>
+    <tableColumn id="3" xr3:uid="{7883BA0C-31AD-2642-B207-2F1C9F10DCF0}" name="path"/>
+    <tableColumn id="4" xr3:uid="{1E92DD59-D455-804F-BF6A-F632B7EDFD84}" name="filename_cleaned"/>
+    <tableColumn id="5" xr3:uid="{843E5AF8-5C67-FA45-837B-EA362EFA107E}" name="path_pattern"/>
+    <tableColumn id="6" xr3:uid="{78E70CFE-8C26-C644-8B91-69082C106EC6}" name="filename_pattern"/>
+    <tableColumn id="7" xr3:uid="{90F3DCEA-FE01-2542-B8B5-D5E518801B39}" name="studio"/>
+    <tableColumn id="8" xr3:uid="{8D77AD12-8A38-C440-AFA3-4C507ED03E92}" name="title"/>
+    <tableColumn id="9" xr3:uid="{13155B3D-C8CF-5246-9EB5-76A3530C12DA}" name="performers"/>
+    <tableColumn id="10" xr3:uid="{7BF5A886-0B23-4A45-AA1E-DD2242400829}" name="date"/>
+    <tableColumn id="11" xr3:uid="{88730EC0-616C-AF42-A241-3EFC40CACE51}" name="studio_code"/>
+    <tableColumn id="12" xr3:uid="{5B177E8A-2B38-924C-A672-48120CE13696}" name="sequence"/>
+    <tableColumn id="13" xr3:uid="{88ACF96A-5726-1B4D-A715-4D2919F75376}" name="group"/>
+    <tableColumn id="14" xr3:uid="{FFE9D10E-25FB-1543-82F7-2256A0074805}" name="unlabeled_path_tokens"/>
+    <tableColumn id="15" xr3:uid="{DA19A5A1-0DF7-B248-B0C0-A49B79CA0898}" name="unlabeled_filename_tokens"/>
+    <tableColumn id="16" xr3:uid="{7580C2B5-011C-EE41-844C-DE6A82CFB64C}" name="match_stats"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -817,9 +863,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="60.1640625" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="64.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -948,45 +1001,48 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" t="s">
-        <v>43</v>
+        <v>127</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5">
+        <v>2005</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="P6" t="s">
         <v>30</v>
@@ -994,22 +1050,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
         <v>47</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
       </c>
       <c r="P7" t="s">
         <v>30</v>
@@ -1017,22 +1073,22 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="P8" t="s">
         <v>30</v>
@@ -1040,22 +1096,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="P9" t="s">
         <v>30</v>
@@ -1063,22 +1119,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I10" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="P10" t="s">
         <v>30</v>
@@ -1086,42 +1142,42 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="P11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K12">
         <v>3190</v>
@@ -1132,118 +1188,109 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
-      </c>
-      <c r="N13" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="P13" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" t="s">
         <v>82</v>
       </c>
-      <c r="F14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I14" t="s">
-        <v>92</v>
-      </c>
-      <c r="N14" t="s">
-        <v>93</v>
-      </c>
       <c r="P14" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N15" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="P15" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H16" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="P16" t="s">
         <v>23</v>
@@ -1251,22 +1298,22 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G17" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I17" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="K17">
         <v>161</v>
@@ -1277,104 +1324,95 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="I18" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="K18" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="L18" t="s">
-        <v>117</v>
-      </c>
-      <c r="N18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="P18" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
-      </c>
-      <c r="N19" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="P19" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G20" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="H20" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="L20" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="M20" t="s">
-        <v>134</v>
-      </c>
-      <c r="N20" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="P20" t="s">
         <v>136</v>
@@ -1382,37 +1420,34 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F21" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="G21" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I21" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="L21" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="M21" t="s">
-        <v>143</v>
-      </c>
-      <c r="N21" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="P21" t="s">
         <v>136</v>
@@ -1420,5 +1455,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>